<commit_message>
Process reruned and output file updated
</commit_message>
<xml_diff>
--- a/Data/Output/output_vendor.xlsx
+++ b/Data/Output/output_vendor.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meeno\Desktop\Robotic Process Automation\UiPath RPA Developer Advanced Certification\Practice Exam\ACME Vendor Check\Data\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{032BF560-35A0-4DE2-9112-AE58A732764C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA55E041-CC9F-4240-9222-5A0702FE2E5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8964" xr2:uid="{341D64EB-1CE8-479C-8BA0-57B7EA7B807E}"/>
+    <workbookView xWindow="30990" yWindow="4965" windowWidth="17280" windowHeight="8970" xr2:uid="{341D64EB-1CE8-479C-8BA0-57B7EA7B807E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="38">
   <si>
     <t>Vendor</t>
   </si>
@@ -490,11 +490,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82F17A60-23A4-4247-BC9B-B0F4F75B99A6}">
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -649,414 +654,6 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" t="s">
-        <v>23</v>
-      </c>
-      <c r="D14" t="s">
-        <v>24</v>
-      </c>
-      <c r="E14" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" t="s">
-        <v>28</v>
-      </c>
-      <c r="D15" t="s">
-        <v>16</v>
-      </c>
-      <c r="E15" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" t="s">
-        <v>31</v>
-      </c>
-      <c r="D16" t="s">
-        <v>32</v>
-      </c>
-      <c r="E16" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>34</v>
-      </c>
-      <c r="B17" t="s">
-        <v>35</v>
-      </c>
-      <c r="C17" t="s">
-        <v>36</v>
-      </c>
-      <c r="D17" t="s">
-        <v>37</v>
-      </c>
-      <c r="E17" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>5</v>
-      </c>
-      <c r="B18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18" t="s">
-        <v>7</v>
-      </c>
-      <c r="D18" t="s">
-        <v>8</v>
-      </c>
-      <c r="E18" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>10</v>
-      </c>
-      <c r="B19" t="s">
-        <v>11</v>
-      </c>
-      <c r="C19" t="s">
-        <v>12</v>
-      </c>
-      <c r="D19" t="s">
-        <v>8</v>
-      </c>
-      <c r="E19" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>13</v>
-      </c>
-      <c r="B20" t="s">
-        <v>14</v>
-      </c>
-      <c r="C20" t="s">
-        <v>15</v>
-      </c>
-      <c r="D20" t="s">
-        <v>16</v>
-      </c>
-      <c r="E20" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>18</v>
-      </c>
-      <c r="B21" t="s">
-        <v>19</v>
-      </c>
-      <c r="C21" t="s">
-        <v>20</v>
-      </c>
-      <c r="D21" t="s">
-        <v>8</v>
-      </c>
-      <c r="E21" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>21</v>
-      </c>
-      <c r="B22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C22" t="s">
-        <v>23</v>
-      </c>
-      <c r="D22" t="s">
-        <v>24</v>
-      </c>
-      <c r="E22" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>26</v>
-      </c>
-      <c r="B23" t="s">
-        <v>27</v>
-      </c>
-      <c r="C23" t="s">
-        <v>28</v>
-      </c>
-      <c r="D23" t="s">
-        <v>16</v>
-      </c>
-      <c r="E23" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>29</v>
-      </c>
-      <c r="B24" t="s">
-        <v>30</v>
-      </c>
-      <c r="C24" t="s">
-        <v>31</v>
-      </c>
-      <c r="D24" t="s">
-        <v>32</v>
-      </c>
-      <c r="E24" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>34</v>
-      </c>
-      <c r="B25" t="s">
-        <v>35</v>
-      </c>
-      <c r="C25" t="s">
-        <v>36</v>
-      </c>
-      <c r="D25" t="s">
-        <v>37</v>
-      </c>
-      <c r="E25" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>5</v>
-      </c>
-      <c r="B26" t="s">
-        <v>6</v>
-      </c>
-      <c r="C26" t="s">
-        <v>7</v>
-      </c>
-      <c r="D26" t="s">
-        <v>8</v>
-      </c>
-      <c r="E26" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>10</v>
-      </c>
-      <c r="B27" t="s">
-        <v>11</v>
-      </c>
-      <c r="C27" t="s">
-        <v>12</v>
-      </c>
-      <c r="D27" t="s">
-        <v>8</v>
-      </c>
-      <c r="E27" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>13</v>
-      </c>
-      <c r="B28" t="s">
-        <v>14</v>
-      </c>
-      <c r="C28" t="s">
-        <v>15</v>
-      </c>
-      <c r="D28" t="s">
-        <v>16</v>
-      </c>
-      <c r="E28" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>18</v>
-      </c>
-      <c r="B29" t="s">
-        <v>19</v>
-      </c>
-      <c r="C29" t="s">
-        <v>20</v>
-      </c>
-      <c r="D29" t="s">
-        <v>8</v>
-      </c>
-      <c r="E29" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>21</v>
-      </c>
-      <c r="B30" t="s">
-        <v>22</v>
-      </c>
-      <c r="C30" t="s">
-        <v>23</v>
-      </c>
-      <c r="D30" t="s">
-        <v>24</v>
-      </c>
-      <c r="E30" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B31" t="s">
-        <v>27</v>
-      </c>
-      <c r="C31" t="s">
-        <v>28</v>
-      </c>
-      <c r="D31" t="s">
-        <v>16</v>
-      </c>
-      <c r="E31" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>29</v>
-      </c>
-      <c r="B32" t="s">
-        <v>30</v>
-      </c>
-      <c r="C32" t="s">
-        <v>31</v>
-      </c>
-      <c r="D32" t="s">
-        <v>32</v>
-      </c>
-      <c r="E32" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>34</v>
-      </c>
-      <c r="B33" t="s">
-        <v>35</v>
-      </c>
-      <c r="C33" t="s">
-        <v>36</v>
-      </c>
-      <c r="D33" t="s">
-        <v>37</v>
-      </c>
-      <c r="E33" t="s">
-        <v>17</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>